<commit_message>
delete the configure files
</commit_message>
<xml_diff>
--- a/other/phone.xlsx
+++ b/other/phone.xlsx
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1719,6 +1719,58 @@
         <v>0.38</v>
       </c>
       <c r="M39">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1">
+        <v>42036</v>
+      </c>
+      <c r="B40">
+        <v>51.73</v>
+      </c>
+      <c r="C40">
+        <v>17</v>
+      </c>
+      <c r="D40">
+        <v>34.729999999999997</v>
+      </c>
+      <c r="H40">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="I40">
+        <v>18.98</v>
+      </c>
+      <c r="J40">
+        <v>7.89</v>
+      </c>
+      <c r="K40">
+        <v>6.65</v>
+      </c>
+      <c r="M40">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1">
+        <v>42064</v>
+      </c>
+      <c r="B41">
+        <v>53.32</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41">
+        <v>36.32</v>
+      </c>
+      <c r="H41">
+        <v>3.6</v>
+      </c>
+      <c r="I41">
+        <v>32.72</v>
+      </c>
+      <c r="M41">
         <v>71</v>
       </c>
     </row>

</xml_diff>